<commit_message>
Working with Data: Non-Relational Databases - Task complete
</commit_message>
<xml_diff>
--- a/2-Trabajar-con-datos/6-BD-No-Relacionales/CocaColaCo.xlsx
+++ b/2-Trabajar-con-datos/6-BD-No-Relacionales/CocaColaCo.xlsx
@@ -1,38 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasmineg\projects\Data-Science-For-Beginners\2-Working-With-Data\06-non-relational\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\LAUNCH X\Web-dev\Projects\Data-Sciencie\2-Trabajar-con-datos\6-BD-No-Relacionales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291207B9-196B-4B03-8D34-EB4EEEE77362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA527C3-6C46-4312-A239-EB654A50DC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COCA COLA CO" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Profit &amp; Loss statement</t>
   </si>
@@ -77,9 +65,6 @@
   </si>
   <si>
     <t>Average Gross Profit from FY '09 TO FY '18</t>
-  </si>
-  <si>
-    <t>Put Formula Here</t>
   </si>
   <si>
     <t>Net operating revenues</t>
@@ -88,9 +73,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -154,24 +139,51 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{B498FFF8-1418-4A3E-9A3B-E7C3DC5142CD}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -473,13 +485,13 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="134.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -525,37 +537,37 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
         <v>30990</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>35119</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>46542</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>48017</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>46854</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>45998</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>44294</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>41863</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>35410</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>31856</v>
       </c>
     </row>
@@ -563,34 +575,34 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>11088</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>12693</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>18215</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>19053</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>18421</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>17889</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>17482</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>16465</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>13255</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>11770</v>
       </c>
     </row>
@@ -598,36 +610,85 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>19902</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>22426</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>28327</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>28964</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>28433</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f>H4-H5</f>
         <v>28109</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="I6" s="5">
+        <f t="shared" ref="I6:L6" si="0">I4-I5</f>
+        <v>26812</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>25398</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="0"/>
+        <v>22155</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" si="0"/>
+        <v>20086</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
+      <c r="C8" s="6">
+        <f>AVERAGE(C4:C5)</f>
+        <v>21039</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" ref="D8:L8" si="1">AVERAGE(D4:D5)</f>
+        <v>23906</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>32378.5</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>33535</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>32637.5</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>31943.5</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>30888</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>29164</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="1"/>
+        <v>24332.5</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="1"/>
+        <v>21813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>